<commit_message>
testng.xml and POM updated with plugins
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -649,7 +649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -659,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>

</xml_diff>